<commit_message>
[#2296119] Restore the CQL Essentials profile
</commit_message>
<xml_diff>
--- a/src/main/resources/API4KP-Registry.xlsx
+++ b/src/main/resources/API4KP-Registry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\API4KB\api4kbs\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AF7BA8-CA1E-4292-B9BF-9C13179CF835}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C74FA8-64EF-48C8-BC24-6165A2A49430}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28170" windowHeight="14378" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28170" windowHeight="14378" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Languages" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="537">
   <si>
     <t>Language</t>
   </si>
@@ -1626,6 +1626,27 @@
   </si>
   <si>
     <t>http://www.omg.org/spec/DOL/DOL-terms/</t>
+  </si>
+  <si>
+    <t>CQLEssentials</t>
+  </si>
+  <si>
+    <t>http://kmdp.mayo.edu/CQL/1.3/essentials</t>
+  </si>
+  <si>
+    <t>kmdp-prof</t>
+  </si>
+  <si>
+    <t>CQL Essentials</t>
+  </si>
+  <si>
+    <t>cql-exx</t>
+  </si>
+  <si>
+    <t>Essential elements of CQL, scoped to simple expressions, used to evalute context variables</t>
+  </si>
+  <si>
+    <t>http://cql.hl7.org</t>
   </si>
 </sst>
 </file>
@@ -3161,10 +3182,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3496,6 +3517,35 @@
       </c>
       <c r="J11" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>530</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>531</v>
+      </c>
+      <c r="C12" t="s">
+        <v>532</v>
+      </c>
+      <c r="E12" t="s">
+        <v>533</v>
+      </c>
+      <c r="F12" t="s">
+        <v>533</v>
+      </c>
+      <c r="G12" t="s">
+        <v>534</v>
+      </c>
+      <c r="H12" t="s">
+        <v>535</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>536</v>
+      </c>
+      <c r="J12" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -5388,7 +5438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>